<commit_message>
Moved scenes to xml
</commit_message>
<xml_diff>
--- a/Task_Click_Point/Sprites.xlsx
+++ b/Task_Click_Point/Sprites.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>spriteType</t>
   </si>
@@ -55,6 +55,9 @@
     <t>yPos</t>
   </si>
   <si>
+    <t>scene</t>
+  </si>
+  <si>
     <t>Character</t>
   </si>
   <si>
@@ -103,6 +106,9 @@
     <t>Indiana Jones</t>
   </si>
   <si>
+    <t>Johhnnyyy</t>
+  </si>
+  <si>
     <t>Rocket</t>
   </si>
   <si>
@@ -203,9 +209,6 @@
   </si>
   <si>
     <t>Sprites\\letter9.png</t>
-  </si>
-  <si>
-    <t>Johhnnyyy</t>
   </si>
 </sst>
 </file>
@@ -263,7 +266,7 @@
 
 <file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
 <MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema2">
+  <Schema ID="Schema1">
     <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
       <xsd:element nillable="true" name="data">
         <xsd:complexType>
@@ -278,6 +281,7 @@
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="spriteHeight" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="xPos" form="unqualified"/>
                   <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="yPos" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:integer" name="scene" form="unqualified"/>
                 </xsd:sequence>
               </xsd:complexType>
             </xsd:element>
@@ -286,36 +290,39 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
-  <Map ID="2" Name="data_Zuordnung" RootElement="data" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+  <Map ID="1" Name="data_Zuordnung" RootElement="data" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
     <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:G26" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:G26"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:H26" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:H26"/>
+  <tableColumns count="8">
     <tableColumn id="1" uniqueName="spriteType" name="spriteType">
-      <xmlColumnPr mapId="2" xpath="/data/Sprite/spriteType" xmlDataType="string"/>
+      <xmlColumnPr mapId="1" xpath="/data/Sprite/spriteType" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="name" name="name">
-      <xmlColumnPr mapId="2" xpath="/data/Sprite/name" xmlDataType="string"/>
+      <xmlColumnPr mapId="1" xpath="/data/Sprite/name" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="location" name="location">
-      <xmlColumnPr mapId="2" xpath="/data/Sprite/location" xmlDataType="string"/>
+      <xmlColumnPr mapId="1" xpath="/data/Sprite/location" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="4" uniqueName="spriteWidth" name="spriteWidth">
-      <xmlColumnPr mapId="2" xpath="/data/Sprite/spriteWidth" xmlDataType="integer"/>
+      <xmlColumnPr mapId="1" xpath="/data/Sprite/spriteWidth" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="5" uniqueName="spriteHeight" name="spriteHeight">
-      <xmlColumnPr mapId="2" xpath="/data/Sprite/spriteHeight" xmlDataType="integer"/>
+      <xmlColumnPr mapId="1" xpath="/data/Sprite/spriteHeight" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="6" uniqueName="xPos" name="xPos">
-      <xmlColumnPr mapId="2" xpath="/data/Sprite/xPos" xmlDataType="integer"/>
+      <xmlColumnPr mapId="1" xpath="/data/Sprite/xPos" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="7" uniqueName="yPos" name="yPos">
-      <xmlColumnPr mapId="2" xpath="/data/Sprite/yPos" xmlDataType="integer"/>
+      <xmlColumnPr mapId="1" xpath="/data/Sprite/yPos" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="8" uniqueName="scene" name="scene">
+      <xmlColumnPr mapId="1" xpath="/data/Sprite/scene" xmlDataType="integer"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -585,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,9 +606,10 @@
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -623,16 +631,19 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D2">
         <v>32</v>
@@ -646,16 +657,19 @@
       <c r="G2">
         <v>250</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <v>32</v>
@@ -669,16 +683,19 @@
       <c r="G3">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>32</v>
@@ -692,16 +709,19 @@
       <c r="G4">
         <v>230</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>32</v>
@@ -715,16 +735,19 @@
       <c r="G5">
         <v>220</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>32</v>
@@ -738,16 +761,19 @@
       <c r="G6">
         <v>250</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D7">
         <v>40</v>
@@ -761,16 +787,19 @@
       <c r="G7">
         <v>240</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D8">
         <v>32</v>
@@ -784,16 +813,19 @@
       <c r="G8">
         <v>240</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D9">
         <v>96</v>
@@ -807,16 +839,19 @@
       <c r="G9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>40</v>
@@ -830,16 +865,19 @@
       <c r="G10">
         <v>190</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D11">
         <v>32</v>
@@ -853,16 +891,19 @@
       <c r="G11">
         <v>190</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D12">
         <v>32</v>
@@ -876,16 +917,19 @@
       <c r="G12">
         <v>250</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D13">
         <v>40</v>
@@ -899,16 +943,19 @@
       <c r="G13">
         <v>250</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>32</v>
@@ -922,16 +969,19 @@
       <c r="G14">
         <v>250</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D15">
         <v>32</v>
@@ -945,16 +995,19 @@
       <c r="G15">
         <v>190</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D16">
         <v>32</v>
@@ -968,16 +1021,19 @@
       <c r="G16">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D17">
         <v>32</v>
@@ -991,16 +1047,19 @@
       <c r="G17">
         <v>300</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1014,16 +1073,19 @@
       <c r="G18">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -1037,16 +1099,19 @@
       <c r="G19">
         <v>75</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -1060,16 +1125,19 @@
       <c r="G20">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1083,16 +1151,19 @@
       <c r="G21">
         <v>75</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -1106,16 +1177,19 @@
       <c r="G22">
         <v>136</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1129,16 +1203,19 @@
       <c r="G23">
         <v>136</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1152,16 +1229,19 @@
       <c r="G24">
         <v>136</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1175,16 +1255,19 @@
       <c r="G25">
         <v>136</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -1197,6 +1280,9 @@
       </c>
       <c r="G26">
         <v>199</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>